<commit_message>
update fichier excel Signed-off-by: Timothee <t1m95.tb@gmail.com>
</commit_message>
<xml_diff>
--- a/doc/Projet Jeu de Dames.xlsx
+++ b/doc/Projet Jeu de Dames.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="90" windowWidth="20115" windowHeight="8250"/>
+    <workbookView xWindow="600" yWindow="90" windowWidth="20115" windowHeight="8250" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Présentation" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="Cahier des charges" sheetId="2" r:id="rId2"/>
+    <sheet name="Algorithmes" sheetId="3" r:id="rId3"/>
+    <sheet name="Classes" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
   <si>
     <t>Régles du  jeu de Dames :</t>
   </si>
@@ -46,6 +47,165 @@
   </si>
   <si>
     <t>algorithme de mouvements possible des pions (moyen)</t>
+  </si>
+  <si>
+    <t>Damier</t>
+  </si>
+  <si>
+    <t>100 cases (50 de couleur et 50 cases blanches)</t>
+  </si>
+  <si>
+    <t>en dimension 10x10 (carré)</t>
+  </si>
+  <si>
+    <t>Pions</t>
+  </si>
+  <si>
+    <t>Pion normal</t>
+  </si>
+  <si>
+    <t>Reine (empilement de deux pions)</t>
+  </si>
+  <si>
+    <t>Types</t>
+  </si>
+  <si>
+    <t>Couleurs</t>
+  </si>
+  <si>
+    <t>Emplacement initial</t>
+  </si>
+  <si>
+    <t>Pions blanc</t>
+  </si>
+  <si>
+    <t>En haut</t>
+  </si>
+  <si>
+    <t>Pions noirs</t>
+  </si>
+  <si>
+    <t>En bas</t>
+  </si>
+  <si>
+    <t>Sur les cases de couleur</t>
+  </si>
+  <si>
+    <t>Quantité</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Note : les deux lignes centrales sont vides</t>
+  </si>
+  <si>
+    <t>Même quantité initiale pour les deux camps</t>
+  </si>
+  <si>
+    <t>4x5 = 20 pions</t>
+  </si>
+  <si>
+    <t>Composition</t>
+  </si>
+  <si>
+    <t>Positionnement</t>
+  </si>
+  <si>
+    <t>Le damier doit être placé de sorte que la première case de gauche, pour chaque joueur, soit une case foncée</t>
+  </si>
+  <si>
+    <t>Sur 3 lignes</t>
+  </si>
+  <si>
+    <t>Blanc</t>
+  </si>
+  <si>
+    <t>Noir</t>
+  </si>
+  <si>
+    <t>Règles de déplacement :</t>
+  </si>
+  <si>
+    <t>Pion</t>
+  </si>
+  <si>
+    <t>Le pion blanc se déplacement en 1er</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Si case vide en face (max de 2)</t>
+  </si>
+  <si>
+    <t>Changement du pion en dame (new Dame)</t>
+  </si>
+  <si>
+    <t>Dame</t>
+  </si>
+  <si>
+    <t>Le pion adverse est perdu</t>
+  </si>
+  <si>
+    <t>Si une pièce est sélectionnée, alors c'est elle qu'il faut jouer</t>
+  </si>
+  <si>
+    <t>Possibilité de le "manger"</t>
+  </si>
+  <si>
+    <t>Si pion adverse mangé</t>
+  </si>
+  <si>
+    <t>Déplacement en avant seulement ET en diagonal (cases couleur)</t>
+  </si>
+  <si>
+    <t>L'adversaire perd un pion</t>
+  </si>
+  <si>
+    <t>Recusivité "Si pion adverse accessible"</t>
+  </si>
+  <si>
+    <t>Si pion adverse dans une diagonale ET au moins une case vide à l'opposé</t>
+  </si>
+  <si>
+    <t>Si aucun pion adverse dans la diagonale</t>
+  </si>
+  <si>
+    <t>Si le pion arrive à la dernière ligne en face</t>
+  </si>
+  <si>
+    <t>Si le pion se fait manger</t>
+  </si>
+  <si>
+    <t>Le pion disparait</t>
+  </si>
+  <si>
+    <t>Une partie est perdue dans le cas inverse</t>
+  </si>
+  <si>
+    <t>Une partie est gagnée quand tous les pions adverses ont été "mangés"</t>
+  </si>
+  <si>
+    <t>Récursivité "Si pion adverse dans une diagonale ET au moins une case vide à l'opposé"</t>
+  </si>
+  <si>
+    <t>Déplacement sur la case de son choix</t>
+  </si>
+  <si>
+    <t>Si la dame se fait manger</t>
+  </si>
+  <si>
+    <t>Si pion adverse accessible ET case vide à l'opposé</t>
+  </si>
+  <si>
+    <t>La dame redevient pion (repise comportement pion)</t>
+  </si>
+  <si>
+    <t>La dame se déplace sur une des cases libres à l'opposé</t>
+  </si>
+  <si>
+    <t>Le pion se déplace sur un case libre juste à l'opposé</t>
   </si>
 </sst>
 </file>
@@ -112,7 +272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -120,6 +280,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -424,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,11 +634,11 @@
       <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="K2" s="1"/>
       <c r="M2" t="s">
         <v>0</v>
       </c>
@@ -489,11 +650,11 @@
       <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="J3" s="1"/>
       <c r="M3" t="s">
         <v>4</v>
       </c>
@@ -502,11 +663,11 @@
       <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="K4" s="1"/>
       <c r="M4" t="s">
         <v>5</v>
       </c>
@@ -515,11 +676,11 @@
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="J5" s="1"/>
       <c r="M5" s="4" t="s">
         <v>2</v>
       </c>
@@ -528,11 +689,11 @@
       <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="K6" s="1"/>
       <c r="M6" t="s">
         <v>6</v>
       </c>
@@ -541,11 +702,11 @@
       <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="J7" s="1"/>
       <c r="M7" t="s">
         <v>7</v>
       </c>
@@ -554,11 +715,11 @@
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="J8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="K8" s="1"/>
       <c r="M8" t="s">
         <v>8</v>
       </c>
@@ -567,11 +728,11 @@
       <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="J9" s="1"/>
       <c r="M9" t="s">
         <v>9</v>
       </c>
@@ -580,21 +741,21 @@
       <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:15" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="J11" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -607,15 +768,304 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="C31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="C33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C35" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C36" s="5"/>
+      <c r="D36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C37" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C38" s="5"/>
+      <c r="D38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C39" s="5"/>
+      <c r="D39" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C40" s="5"/>
+      <c r="E40" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C41" s="5"/>
+      <c r="E41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C42" s="5"/>
+      <c r="E42" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C43" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C45" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C49" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D51" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C55" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D56" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C57" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -629,4 +1079,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Signed-off-by: Timothee <t1m95.tb@gmail.com> Signed-off-by: t1m0t <t1m95.tb@gmail.com>
</commit_message>
<xml_diff>
--- a/doc/Projet Jeu de Dames.xlsx
+++ b/doc/Projet Jeu de Dames.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="90" windowWidth="20115" windowHeight="8250" activeTab="1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="78">
   <si>
     <t>Régles du  jeu de Dames :</t>
   </si>
@@ -145,24 +145,12 @@
     <t>Dame</t>
   </si>
   <si>
-    <t>Le pion adverse est perdu</t>
-  </si>
-  <si>
     <t>Si une pièce est sélectionnée, alors c'est elle qu'il faut jouer</t>
   </si>
   <si>
-    <t>Possibilité de le "manger"</t>
-  </si>
-  <si>
-    <t>Si pion adverse mangé</t>
-  </si>
-  <si>
     <t>Déplacement en avant seulement ET en diagonal (cases couleur)</t>
   </si>
   <si>
-    <t>L'adversaire perd un pion</t>
-  </si>
-  <si>
     <t>Recusivité "Si pion adverse accessible"</t>
   </si>
   <si>
@@ -178,9 +166,6 @@
     <t>Si le pion se fait manger</t>
   </si>
   <si>
-    <t>Le pion disparait</t>
-  </si>
-  <si>
     <t>Une partie est perdue dans le cas inverse</t>
   </si>
   <si>
@@ -206,6 +191,66 @@
   </si>
   <si>
     <t>Le pion se déplace sur un case libre juste à l'opposé</t>
+  </si>
+  <si>
+    <t>Le pion disparait du damier</t>
+  </si>
+  <si>
+    <t>Obligation de le "manger"</t>
+  </si>
+  <si>
+    <t>L'adversaire perd le pion "sauté"</t>
+  </si>
+  <si>
+    <t>Si plusieurs choix, le choix qui prend le plus de pion est choisi (dame = pion ici)</t>
+  </si>
+  <si>
+    <t>Si refus</t>
+  </si>
+  <si>
+    <t>Le pion reviens à sa position initiale</t>
+  </si>
+  <si>
+    <t>Si choix du joueur non conforme, possibilité de refuser le mouvement par l'adversaire</t>
+  </si>
+  <si>
+    <t>Si validation</t>
+  </si>
+  <si>
+    <t>Validation automatique</t>
+  </si>
+  <si>
+    <t>Si choix du joueur conforme</t>
+  </si>
+  <si>
+    <t>Si mouvement réellement non conforme</t>
+  </si>
+  <si>
+    <t>Afficher "refus impossible"</t>
+  </si>
+  <si>
+    <t>Afficher "accepter" (pendant 5 secondes)</t>
+  </si>
+  <si>
+    <t>L'adversaire perd le(s) pion(s) "sauté(s)"</t>
+  </si>
+  <si>
+    <t>Mouvement(s) du joureurs (dans la totalité)</t>
+  </si>
+  <si>
+    <t>choix[#choix]</t>
+  </si>
+  <si>
+    <t>Quand un pion est bougé définitivement, re-calculer les mouvement possibles de ses pions (du genre updatePossibleMooves())</t>
+  </si>
+  <si>
+    <t>Les mouvements possibles se feront sous cette forme pour chaque pions</t>
+  </si>
+  <si>
+    <t>Sinon ( à voir  pour donner une pénalité )</t>
+  </si>
+  <si>
+    <t>Si plusieurs choix, le choix qui prend le plus de pion doit être privilégié (pion = dame)</t>
   </si>
 </sst>
 </file>
@@ -294,6 +339,523 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="ZoneTexte 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="847725" y="295275"/>
+          <a:ext cx="1571625" cy="2609850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Classe Damier</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="ZoneTexte 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3886200" y="3438525"/>
+          <a:ext cx="1571625" cy="2609850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Classe Pion</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="ZoneTexte 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3924300" y="333375"/>
+          <a:ext cx="1571625" cy="2609850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Classe Cases</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="ZoneTexte 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6334125" y="5686425"/>
+          <a:ext cx="1571625" cy="2609850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Classe PDame</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="ZoneTexte 5"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6391275" y="2647950"/>
+          <a:ext cx="1571625" cy="2609850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Classe PBasic</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="ZoneTexte 8"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9248775" y="5657850"/>
+          <a:ext cx="1571625" cy="2609850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Classe DMoove</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="ZoneTexte 9"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12077700" y="4219575"/>
+          <a:ext cx="1571625" cy="2609850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Classe Moove</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="ZoneTexte 10"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9286875" y="2628900"/>
+          <a:ext cx="1571625" cy="2609850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Classe PMoove</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -586,7 +1148,7 @@
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,145 +1484,252 @@
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="C32" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="C33" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C35" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C36" s="5"/>
       <c r="D36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C37" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C38" s="5"/>
       <c r="D38" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C39" s="5"/>
       <c r="D39" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="F43" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="H45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="G46" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="H47" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="F48" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="G49" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="G50" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C51" s="5"/>
+      <c r="G51" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C52" s="5"/>
+      <c r="E52" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C53" s="5"/>
+      <c r="F53" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C54" s="5"/>
+      <c r="F54" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C55" s="5"/>
+      <c r="F55" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C56" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D57" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C58" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C62" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="5"/>
-      <c r="E40" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="5"/>
-      <c r="E41" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C42" s="5"/>
-      <c r="E42" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="5" t="s">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D64" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="5" t="s">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C68" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D46" t="s">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C70" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C49" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D50" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D51" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E52" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E53" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="E54" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C55" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D56" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C57" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
-        <v>60</v>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1085,10 +1754,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tim update Signed-off-by: t1m0t <t1m95.tb@gmail.com>
</commit_message>
<xml_diff>
--- a/doc/Projet Jeu de Dames.xlsx
+++ b/doc/Projet Jeu de Dames.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="90" windowWidth="20115" windowHeight="8250" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="90" windowWidth="20115" windowHeight="8250" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Présentation" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
   <si>
     <t>Régles du  jeu de Dames :</t>
   </si>
@@ -257,6 +257,15 @@
   </si>
   <si>
     <t>(idem déplacement pion mais les mouvements de la dame sont extensibles)</t>
+  </si>
+  <si>
+    <t>Modes de jeu</t>
+  </si>
+  <si>
+    <t>Contre un personne (ajax)</t>
+  </si>
+  <si>
+    <t>Contre l'IA (algo, pas de mode de difficulté dans un premier temps)</t>
   </si>
 </sst>
 </file>
@@ -589,6 +598,70 @@
           <a:r>
             <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
             <a:t>}</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="ZoneTexte 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="457200" y="5029200"/>
+          <a:ext cx="5915025" cy="2200275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>//calcul des choix possibles</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1587,407 +1660,422 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H83"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="5" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="5" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="5" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="5" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="5" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="5"/>
-      <c r="C30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="C31" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="C32" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="C33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="C34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="C35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="5"/>
+      <c r="C36" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C35" s="5" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C36" s="5"/>
-      <c r="D36" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C37" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C38" s="5"/>
-      <c r="D38" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C39" s="5"/>
       <c r="D39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C40" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C41" s="5"/>
+      <c r="D41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C42" s="5"/>
+      <c r="D42" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C40" s="5"/>
-      <c r="D40" s="5" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C43" s="5"/>
+      <c r="D43" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
-      <c r="F44" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E45" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="H46" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E46" s="5"/>
+      <c r="F46" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
-      <c r="G47" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F47" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
-      <c r="H48" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F48" s="5"/>
+      <c r="G48" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
-      <c r="F49" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F49" s="5"/>
+      <c r="H49" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
-      <c r="G50" t="s">
+      <c r="G50" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="H51" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="F52" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="G53" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C51" s="5"/>
-      <c r="G51" s="5" t="s">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C54" s="5"/>
+      <c r="G54" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="5"/>
-      <c r="E52" s="5" t="s">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C55" s="5"/>
+      <c r="E55" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C53" s="5"/>
-      <c r="F53" t="s">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C56" s="5"/>
+      <c r="F56" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C54" s="5"/>
-      <c r="F54" t="s">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C57" s="5"/>
+      <c r="F57" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C55" s="5"/>
-      <c r="F55" t="s">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C58" s="5"/>
+      <c r="F58" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C56" s="5" t="s">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C59" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D57" t="s">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C58" s="5" t="s">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C61" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B61" s="5" t="s">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C64" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C62" s="5" t="s">
+    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C65" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D63" t="s">
+    <row r="66" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D64" s="5" t="s">
+    <row r="67" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D67" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E65" t="s">
+    <row r="68" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E66" t="s">
+    <row r="69" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E69" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E67" t="s">
+    <row r="70" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E70" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C68" s="5" t="s">
+    <row r="71" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C71" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D69" t="s">
+    <row r="72" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C70" s="5" t="s">
+    <row r="73" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C73" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D71" t="s">
+    <row r="74" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2001,8 +2089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Tim Update, possibleMooves implemented but has to be cleared (bug) Signed-off-by: t1m0t <t1m95.tb@gmail.com>
</commit_message>
<xml_diff>
--- a/doc/Projet Jeu de Dames.xlsx
+++ b/doc/Projet Jeu de Dames.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="90" windowWidth="20115" windowHeight="8250" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="90" windowWidth="20115" windowHeight="8250" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Présentation" sheetId="1" r:id="rId1"/>
     <sheet name="Cahier des charges" sheetId="2" r:id="rId2"/>
     <sheet name="Algorithmes" sheetId="3" r:id="rId3"/>
     <sheet name="Classes" sheetId="4" r:id="rId4"/>
+    <sheet name="Symfony" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="87">
   <si>
     <t>Régles du  jeu de Dames :</t>
   </si>
@@ -266,13 +267,25 @@
   </si>
   <si>
     <t>Contre l'IA (algo, pas de mode de difficulté dans un premier temps)</t>
+  </si>
+  <si>
+    <t>Token</t>
+  </si>
+  <si>
+    <t>Case 1 : à chaque fin de tour</t>
+  </si>
+  <si>
+    <t>Générer un token : generateCsrfToken(string $intention)</t>
+  </si>
+  <si>
+    <t>Gestion AJAX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,6 +317,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -332,7 +352,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -341,6 +361,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -1662,8 +1685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2089,7 +2112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
@@ -2114,4 +2137,43 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>